<commit_message>
I hate you excel.... ready to start graphing
</commit_message>
<xml_diff>
--- a/Graph_FIle.xlsx
+++ b/Graph_FIle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="49">
   <si>
     <t>FIFO Test Results</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>RR_15</t>
+  </si>
+  <si>
+    <t>Turn Around Times</t>
   </si>
 </sst>
 </file>
@@ -511,20 +514,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -546,8 +552,29 @@
       <c r="G2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>FIFO!B15</f>
         <v>114.2</v>
@@ -561,23 +588,51 @@
         <v>70.2</v>
       </c>
       <c r="D3" s="1">
-        <f>FIFO!E15</f>
-        <v>0</v>
+        <f>RR_5!$B$15</f>
+        <v>163.30000000000001</v>
       </c>
       <c r="E3" s="1">
-        <f>FIFO!F15</f>
-        <v>0</v>
+        <f>RR_10!$B$15</f>
+        <v>152.69999999999999</v>
       </c>
       <c r="F3" s="1">
-        <f>FIFO!G15</f>
-        <v>0</v>
+        <f>RR_15!$B$15</f>
+        <v>146.6</v>
       </c>
       <c r="G3" s="1">
-        <f>FIFO!H15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Stride!$B$15</f>
+        <v>162.30000000000001</v>
+      </c>
+      <c r="J3">
+        <f>FIFO!$B$16</f>
+        <v>145.1</v>
+      </c>
+      <c r="K3">
+        <f>SJF!$B$16</f>
+        <v>101</v>
+      </c>
+      <c r="L3">
+        <f>PESJF!$B$16</f>
+        <v>101.1</v>
+      </c>
+      <c r="M3">
+        <f>RR_5!$B$16</f>
+        <v>194.2</v>
+      </c>
+      <c r="N3">
+        <f>RR_10!$B$16</f>
+        <v>183.6</v>
+      </c>
+      <c r="O3">
+        <f>RR_15!$B$16</f>
+        <v>177.5</v>
+      </c>
+      <c r="P3">
+        <f>Stride!$B$16</f>
+        <v>193.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>FIFO!B30</f>
         <v>134.6</v>
@@ -591,23 +646,51 @@
         <v>83.6</v>
       </c>
       <c r="D4">
-        <f>FIFO!E30</f>
-        <v>0</v>
+        <f>RR_5!$B$30</f>
+        <v>217.7</v>
       </c>
       <c r="E4">
-        <f>FIFO!F30</f>
-        <v>0</v>
+        <f>RR_10!$B$30</f>
+        <v>189.5</v>
       </c>
       <c r="F4">
-        <f>FIFO!G30</f>
-        <v>0</v>
+        <f>RR_15!$B$30</f>
+        <v>184</v>
       </c>
       <c r="G4">
-        <f>FIFO!H30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+        <f>Stride!$B$30</f>
+        <v>184.3</v>
+      </c>
+      <c r="J4">
+        <f>FIFO!$B$31</f>
+        <v>165.3</v>
+      </c>
+      <c r="K4">
+        <f>SJF!$B$31</f>
+        <v>121.5</v>
+      </c>
+      <c r="L4">
+        <f>PESJF!$B$31</f>
+        <v>114.3</v>
+      </c>
+      <c r="M4">
+        <f>RR_5!$B$31</f>
+        <v>248.4</v>
+      </c>
+      <c r="N4">
+        <f>RR_10!$B$31</f>
+        <v>220.2</v>
+      </c>
+      <c r="O4">
+        <f>RR_15!$B$31</f>
+        <v>214.7</v>
+      </c>
+      <c r="P4">
+        <f>Stride!$B$31</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>FIFO!B45</f>
         <v>110.6</v>
@@ -617,27 +700,55 @@
         <v>76.5</v>
       </c>
       <c r="C5" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
+        <f>PESJF!$B$45</f>
+        <v>74.400000000000006</v>
       </c>
       <c r="D5" s="1">
-        <f>FIFO!E45</f>
-        <v>0</v>
+        <f>RR_5!$B$45</f>
+        <v>174.2</v>
       </c>
       <c r="E5" s="1">
-        <f>FIFO!F45</f>
-        <v>0</v>
+        <f>RR_10!$B$45</f>
+        <v>164.1</v>
       </c>
       <c r="F5" s="1">
-        <f>FIFO!G45</f>
-        <v>0</v>
+        <f>RR_15!$B$45</f>
+        <v>153.4</v>
       </c>
       <c r="G5" s="1">
-        <f>FIFO!H45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Stride!$B$45</f>
+        <v>216.8</v>
+      </c>
+      <c r="J5">
+        <f>FIFO!$B$46</f>
+        <v>140.80000000000001</v>
+      </c>
+      <c r="K5">
+        <f>SJF!$B$46</f>
+        <v>106.7</v>
+      </c>
+      <c r="L5">
+        <f>PESJF!$B$46</f>
+        <v>104.6</v>
+      </c>
+      <c r="M5">
+        <f>RR_5!$B$46</f>
+        <v>204.4</v>
+      </c>
+      <c r="N5">
+        <f>RR_10!$B$46</f>
+        <v>194.3</v>
+      </c>
+      <c r="O5">
+        <f>RR_15!$B$46</f>
+        <v>183.6</v>
+      </c>
+      <c r="P5">
+        <f>Stride!$B$46</f>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>FIFO!B60</f>
         <v>72.7</v>
@@ -647,27 +758,55 @@
         <v>64.7</v>
       </c>
       <c r="C6">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
+        <f>PESJF!$B$60</f>
+        <v>63.8</v>
       </c>
       <c r="D6">
-        <f>FIFO!E60</f>
-        <v>0</v>
+        <f>RR_5!$B$60</f>
+        <v>147</v>
       </c>
       <c r="E6">
-        <f>FIFO!F60</f>
-        <v>0</v>
+        <f>RR_10!$B$60</f>
+        <v>133.6</v>
       </c>
       <c r="F6">
-        <f>FIFO!G60</f>
-        <v>0</v>
+        <f>RR_15!$B$60</f>
+        <v>119.8</v>
       </c>
       <c r="G6">
-        <f>FIFO!H60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+        <f>Stride!$B$60</f>
+        <v>195.4</v>
+      </c>
+      <c r="J6">
+        <f>FIFO!$B$61</f>
+        <v>101.8</v>
+      </c>
+      <c r="K6">
+        <f>SJF!$B$61</f>
+        <v>93.8</v>
+      </c>
+      <c r="L6">
+        <f>PESJF!$B$61</f>
+        <v>92.9</v>
+      </c>
+      <c r="M6">
+        <f>RR_5!$B$61</f>
+        <v>176.1</v>
+      </c>
+      <c r="N6">
+        <f>RR_10!$B$61</f>
+        <v>162.69999999999999</v>
+      </c>
+      <c r="O6">
+        <f>RR_15!$B$61</f>
+        <v>148.9</v>
+      </c>
+      <c r="P6">
+        <f>Stride!$B$61</f>
+        <v>224.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>FIFO!B75</f>
         <v>122.4</v>
@@ -677,27 +816,55 @@
         <v>76.8</v>
       </c>
       <c r="C7" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
+        <f>PESJF!$B$75</f>
+        <v>64.900000000000006</v>
       </c>
       <c r="D7" s="1">
-        <f>FIFO!E75</f>
-        <v>0</v>
+        <f>RR_5!$B$75</f>
+        <v>148.5</v>
       </c>
       <c r="E7" s="1">
-        <f>FIFO!F75</f>
-        <v>0</v>
+        <f>RR_10!$B$75</f>
+        <v>146.9</v>
       </c>
       <c r="F7" s="1">
-        <f>FIFO!G75</f>
-        <v>0</v>
+        <f>RR_15!$B$75</f>
+        <v>139.6</v>
       </c>
       <c r="G7" s="1">
-        <f>FIFO!H75</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Stride!$B$75</f>
+        <v>154.9</v>
+      </c>
+      <c r="J7">
+        <f>FIFO!$B$76</f>
+        <v>150.6</v>
+      </c>
+      <c r="K7">
+        <f>SJF!$B$76</f>
+        <v>105</v>
+      </c>
+      <c r="L7">
+        <f>PESJF!$B$76</f>
+        <v>93.1</v>
+      </c>
+      <c r="M7">
+        <f>RR_5!$B$76</f>
+        <v>176.7</v>
+      </c>
+      <c r="N7">
+        <f>RR_10!$B$76</f>
+        <v>175.1</v>
+      </c>
+      <c r="O7">
+        <f>RR_15!$B$76</f>
+        <v>167.8</v>
+      </c>
+      <c r="P7">
+        <f>Stride!$B$76</f>
+        <v>183.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>FIFO!B90</f>
         <v>177.9</v>
@@ -706,28 +873,56 @@
         <f>SJF!B90</f>
         <v>145.19999999999999</v>
       </c>
-      <c r="C8">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D8">
-        <f>FIFO!E90</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>FIFO!F90</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>FIFO!G90</f>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>FIFO!H90</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <f>PESJF!$B$90</f>
+        <v>140.9</v>
+      </c>
+      <c r="D8" s="1">
+        <f>RR_5!$B$90</f>
+        <v>318.39999999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <f>RR_10!$B$90</f>
+        <v>320.10000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <f>RR_15!$B$90</f>
+        <v>291.60000000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <f>Stride!$B$90</f>
+        <v>343.8</v>
+      </c>
+      <c r="J8">
+        <f>FIFO!$B$91</f>
+        <v>221.5</v>
+      </c>
+      <c r="K8">
+        <f>SJF!$B$91</f>
+        <v>188.8</v>
+      </c>
+      <c r="L8">
+        <f>PESJF!$B$91</f>
+        <v>184.5</v>
+      </c>
+      <c r="M8">
+        <f>RR_5!$B$91</f>
+        <v>362</v>
+      </c>
+      <c r="N8">
+        <f>RR_10!$B$91</f>
+        <v>363.7</v>
+      </c>
+      <c r="O8">
+        <f>RR_15!$B$91</f>
+        <v>335.2</v>
+      </c>
+      <c r="P8">
+        <f>Stride!$B$91</f>
+        <v>387.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>FIFO!B105</f>
         <v>179.6</v>
@@ -736,28 +931,56 @@
         <f>SJF!B105</f>
         <v>145</v>
       </c>
-      <c r="C9" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D9" s="1">
-        <f>FIFO!E105</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <f>FIFO!F105</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <f>FIFO!G105</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f>FIFO!H105</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>PESJF!$B$105</f>
+        <v>143</v>
+      </c>
+      <c r="D9">
+        <f>RR_5!$B$105</f>
+        <v>312.3</v>
+      </c>
+      <c r="E9">
+        <f>RR_10!$B$105</f>
+        <v>315</v>
+      </c>
+      <c r="F9">
+        <f>RR_15!$B$105</f>
+        <v>291.7</v>
+      </c>
+      <c r="G9">
+        <f>Stride!$B$105</f>
+        <v>331.9</v>
+      </c>
+      <c r="J9">
+        <f>FIFO!$B$106</f>
+        <v>222.8</v>
+      </c>
+      <c r="K9">
+        <f>SJF!$B$106</f>
+        <v>188.2</v>
+      </c>
+      <c r="L9">
+        <f>FIFO!$B$106</f>
+        <v>222.8</v>
+      </c>
+      <c r="M9">
+        <f>RR_5!$B$106</f>
+        <v>355.5</v>
+      </c>
+      <c r="N9">
+        <f>RR_10!$B$106</f>
+        <v>358.2</v>
+      </c>
+      <c r="O9">
+        <f>RR_15!$B$106</f>
+        <v>334.9</v>
+      </c>
+      <c r="P9">
+        <f>Stride!$B$106</f>
+        <v>375.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>FIFO!B120</f>
         <v>90.9</v>
@@ -766,28 +989,56 @@
         <f>SJF!B120</f>
         <v>55.3</v>
       </c>
-      <c r="C10">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D10">
-        <f>FIFO!E120</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>FIFO!F120</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>FIFO!G120</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>FIFO!H120</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <f>PESJF!$B$120</f>
+        <v>54.5</v>
+      </c>
+      <c r="D10" s="1">
+        <f>RR_5!$B$120</f>
+        <v>136.80000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <f>RR_10!$B$120</f>
+        <v>123.8</v>
+      </c>
+      <c r="F10" s="1">
+        <f>RR_15!$B$120</f>
+        <v>110.4</v>
+      </c>
+      <c r="G10" s="1">
+        <f>Stride!$B$120</f>
+        <v>148.9</v>
+      </c>
+      <c r="J10">
+        <f>FIFO!$B$121</f>
+        <v>117.9</v>
+      </c>
+      <c r="K10">
+        <f>SJF!$B$121</f>
+        <v>82.3</v>
+      </c>
+      <c r="L10">
+        <f>PESJF!$B$121</f>
+        <v>81.5</v>
+      </c>
+      <c r="M10">
+        <f>RR_5!$B$121</f>
+        <v>163.80000000000001</v>
+      </c>
+      <c r="N10">
+        <f>RR_10!$B$121</f>
+        <v>150.80000000000001</v>
+      </c>
+      <c r="O10">
+        <f>RR_15!$B$121</f>
+        <v>137.4</v>
+      </c>
+      <c r="P10">
+        <f>Stride!$B$121</f>
+        <v>175.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>FIFO!B135</f>
         <v>136.4</v>
@@ -796,28 +1047,56 @@
         <f>SJF!B135</f>
         <v>104.2</v>
       </c>
-      <c r="C11" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D11" s="1">
-        <f>FIFO!E135</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <f>FIFO!F135</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <f>FIFO!G135</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <f>FIFO!H135</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>PESJF!$B$135</f>
+        <v>104.3</v>
+      </c>
+      <c r="D11">
+        <f>RR_5!$B$135</f>
+        <v>265.3</v>
+      </c>
+      <c r="E11">
+        <f>RR_10!$B$135</f>
+        <v>232.3</v>
+      </c>
+      <c r="F11">
+        <f>RR_15!$B$135</f>
+        <v>212.8</v>
+      </c>
+      <c r="G11">
+        <f>Stride!$B$135</f>
+        <v>225.3</v>
+      </c>
+      <c r="J11">
+        <f>FIFO!$B$136</f>
+        <v>169.3</v>
+      </c>
+      <c r="K11">
+        <f>SJF!$B$136</f>
+        <v>137.1</v>
+      </c>
+      <c r="L11">
+        <f>PESJF!$B$136</f>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="M11">
+        <f>RR_5!$B$136</f>
+        <v>298.2</v>
+      </c>
+      <c r="N11">
+        <f>RR_10!$B$136</f>
+        <v>265.2</v>
+      </c>
+      <c r="O11">
+        <f>RR_15!$B$136</f>
+        <v>245.7</v>
+      </c>
+      <c r="P11">
+        <f>Stride!$B$136</f>
+        <v>258.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>FIFO!B150</f>
         <v>101.1</v>
@@ -826,28 +1105,56 @@
         <f>SJF!B150</f>
         <v>72</v>
       </c>
-      <c r="C12">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D12">
-        <f>FIFO!E150</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>FIFO!F150</f>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f>FIFO!G150</f>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>FIFO!H150</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <f>PESJF!$B$150</f>
+        <v>74</v>
+      </c>
+      <c r="D12" s="1">
+        <f>RR_5!$B$150</f>
+        <v>164.1</v>
+      </c>
+      <c r="E12" s="1">
+        <f>RR_10!$B$150</f>
+        <v>154.9</v>
+      </c>
+      <c r="F12" s="1">
+        <f>RR_15!$B$150</f>
+        <v>149.4</v>
+      </c>
+      <c r="G12" s="1">
+        <f>Stride!$B$150</f>
+        <v>165.2</v>
+      </c>
+      <c r="J12">
+        <f>FIFO!$B$151</f>
+        <v>130</v>
+      </c>
+      <c r="K12">
+        <f>SJF!$B$151</f>
+        <v>100.9</v>
+      </c>
+      <c r="L12">
+        <f>PESJF!$B$151</f>
+        <v>102.9</v>
+      </c>
+      <c r="M12">
+        <f>RR_5!$B$151</f>
+        <v>193</v>
+      </c>
+      <c r="N12">
+        <f>RR_10!$B$151</f>
+        <v>183.8</v>
+      </c>
+      <c r="O12">
+        <f>RR_15!$B$151</f>
+        <v>178.3</v>
+      </c>
+      <c r="P12">
+        <f>Stride!$B$151</f>
+        <v>194.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>FIFO!B165</f>
         <v>119.5</v>
@@ -856,28 +1163,56 @@
         <f>SJF!B165</f>
         <v>62.7</v>
       </c>
-      <c r="C13" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D13" s="1">
-        <f>FIFO!E165</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <f>FIFO!F165</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <f>FIFO!G165</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <f>FIFO!H165</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>PESJF!$B$165</f>
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <f>RR_5!$B$165</f>
+        <v>128.30000000000001</v>
+      </c>
+      <c r="E13">
+        <f>RR_10!$B$165</f>
+        <v>145.69999999999999</v>
+      </c>
+      <c r="F13">
+        <f>RR_15!$B$165</f>
+        <v>148.69999999999999</v>
+      </c>
+      <c r="G13">
+        <f>Stride!$B$165</f>
+        <v>133.1</v>
+      </c>
+      <c r="J13">
+        <f>FIFO!$B$166</f>
+        <v>144.6</v>
+      </c>
+      <c r="K13">
+        <f>SJF!$B$166</f>
+        <v>87.8</v>
+      </c>
+      <c r="L13">
+        <f>PESJF!$B$166</f>
+        <v>87.1</v>
+      </c>
+      <c r="M13">
+        <f>RR_5!$B$166</f>
+        <v>153.4</v>
+      </c>
+      <c r="N13">
+        <f>RR_10!$B$166</f>
+        <v>170.8</v>
+      </c>
+      <c r="O13">
+        <f>RR_15!$B$166</f>
+        <v>173.8</v>
+      </c>
+      <c r="P13">
+        <f>Stride!$B$166</f>
+        <v>158.19999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>FIFO!B180</f>
         <v>114.9</v>
@@ -886,28 +1221,56 @@
         <f>SJF!B180</f>
         <v>85.2</v>
       </c>
-      <c r="C14">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D14">
-        <f>FIFO!E180</f>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f>FIFO!F180</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f>FIFO!G180</f>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f>FIFO!H180</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <f>PESJF!$B$180</f>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="D14" s="1">
+        <f>RR_5!$B$180</f>
+        <v>175.2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>RR_10!$B$180</f>
+        <v>176</v>
+      </c>
+      <c r="F14" s="1">
+        <f>RR_15!$B$180</f>
+        <v>158.80000000000001</v>
+      </c>
+      <c r="G14" s="1">
+        <f>Stride!$B$180</f>
+        <v>178.8</v>
+      </c>
+      <c r="J14">
+        <f>FIFO!$B$181</f>
+        <v>145.9</v>
+      </c>
+      <c r="K14">
+        <f>SJF!$B$181</f>
+        <v>116.2</v>
+      </c>
+      <c r="L14">
+        <f>PESJF!$B$181</f>
+        <v>104.9</v>
+      </c>
+      <c r="M14">
+        <f>RR_5!$B$181</f>
+        <v>206.2</v>
+      </c>
+      <c r="N14">
+        <f>RR_10!$B$181</f>
+        <v>207</v>
+      </c>
+      <c r="O14">
+        <f>RR_15!$B$181</f>
+        <v>189.8</v>
+      </c>
+      <c r="P14">
+        <f>Stride!$B$181</f>
+        <v>209.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>FIFO!B195</f>
         <v>143.69999999999999</v>
@@ -916,28 +1279,56 @@
         <f>SJF!B195</f>
         <v>91.6</v>
       </c>
-      <c r="C15" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D15" s="1">
-        <f>FIFO!E195</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <f>FIFO!F195</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <f>FIFO!G195</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <f>FIFO!H195</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>PESJF!$B$195</f>
+        <v>84.4</v>
+      </c>
+      <c r="D15">
+        <f>RR_5!$B$195</f>
+        <v>221.1</v>
+      </c>
+      <c r="E15">
+        <f>RR_10!$B$195</f>
+        <v>201.5</v>
+      </c>
+      <c r="F15">
+        <f>RR_15!$B$195</f>
+        <v>178.2</v>
+      </c>
+      <c r="G15">
+        <f>Stride!$B$195</f>
+        <v>188</v>
+      </c>
+      <c r="J15">
+        <f>FIFO!$B$196</f>
+        <v>174.6</v>
+      </c>
+      <c r="K15">
+        <f>SJF!$B$196</f>
+        <v>122.5</v>
+      </c>
+      <c r="L15">
+        <f>PESJF!$B$196</f>
+        <v>115.3</v>
+      </c>
+      <c r="M15">
+        <f>RR_5!$B$196</f>
+        <v>252</v>
+      </c>
+      <c r="N15">
+        <f>RR_10!$B$196</f>
+        <v>232.4</v>
+      </c>
+      <c r="O15">
+        <f>RR_15!$B$196</f>
+        <v>209.1</v>
+      </c>
+      <c r="P15">
+        <f>Stride!$B$196</f>
+        <v>218.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>FIFO!B210</f>
         <v>111</v>
@@ -946,28 +1337,56 @@
         <f>SJF!B210</f>
         <v>85.6</v>
       </c>
-      <c r="C16">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D16">
-        <f>FIFO!E210</f>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f>FIFO!F210</f>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f>FIFO!G210</f>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f>FIFO!H210</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <f>PESJF!$B$210</f>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D16" s="1">
+        <f>RR_5!$B$210</f>
+        <v>185.4</v>
+      </c>
+      <c r="E16" s="1">
+        <f>RR_10!$B$210</f>
+        <v>161.80000000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <f>RR_15!$B$210</f>
+        <v>161.1</v>
+      </c>
+      <c r="G16" s="1">
+        <f>Stride!$B$210</f>
+        <v>190</v>
+      </c>
+      <c r="J16">
+        <f>FIFO!$B$211</f>
+        <v>139.6</v>
+      </c>
+      <c r="K16">
+        <f>SJF!$B$211</f>
+        <v>114.2</v>
+      </c>
+      <c r="L16">
+        <f>PESJF!$B$211</f>
+        <v>100.5</v>
+      </c>
+      <c r="M16">
+        <f>RR_5!$B$211</f>
+        <v>214</v>
+      </c>
+      <c r="N16">
+        <f>RR_10!$B$211</f>
+        <v>190.4</v>
+      </c>
+      <c r="O16">
+        <f>RR_15!$B$211</f>
+        <v>189.7</v>
+      </c>
+      <c r="P16">
+        <f>Stride!$B$211</f>
+        <v>218.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>FIFO!B225</f>
         <v>146.69999999999999</v>
@@ -976,28 +1395,56 @@
         <f>SJF!B225</f>
         <v>105.7</v>
       </c>
-      <c r="C17" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D17" s="1">
-        <f>FIFO!E225</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <f>FIFO!F225</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <f>FIFO!G225</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <f>FIFO!H225</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>PESJF!$B$225</f>
+        <v>93.4</v>
+      </c>
+      <c r="D17">
+        <f>RR_5!$B$225</f>
+        <v>213.7</v>
+      </c>
+      <c r="E17">
+        <f>RR_10!$B$225</f>
+        <v>209</v>
+      </c>
+      <c r="F17">
+        <f>RR_15!$B$225</f>
+        <v>194.3</v>
+      </c>
+      <c r="G17">
+        <f>Stride!$B$225</f>
+        <v>201.4</v>
+      </c>
+      <c r="J17">
+        <f>FIFO!$B$226</f>
+        <v>181.9</v>
+      </c>
+      <c r="K17">
+        <f>SJF!$B$226</f>
+        <v>140.9</v>
+      </c>
+      <c r="L17">
+        <f>PESJF!$B$226</f>
+        <v>128.6</v>
+      </c>
+      <c r="M17">
+        <f>RR_5!$B$226</f>
+        <v>248.9</v>
+      </c>
+      <c r="N17">
+        <f>RR_10!$B$226</f>
+        <v>244.2</v>
+      </c>
+      <c r="O17">
+        <f>RR_15!$B$226</f>
+        <v>229.5</v>
+      </c>
+      <c r="P17">
+        <f>Stride!$B$226</f>
+        <v>236.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>FIFO!B240</f>
         <v>134.30000000000001</v>
@@ -1006,28 +1453,56 @@
         <f>SJF!B240</f>
         <v>78.400000000000006</v>
       </c>
-      <c r="C18">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D18">
-        <f>FIFO!E240</f>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f>FIFO!F240</f>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f>FIFO!G240</f>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f>FIFO!H240</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <f>PESJF!$B$240</f>
+        <v>70.5</v>
+      </c>
+      <c r="D18" s="1">
+        <f>RR_5!$B$240</f>
+        <v>177.5</v>
+      </c>
+      <c r="E18" s="1">
+        <f>RR_10!$B$240</f>
+        <v>159.19999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <f>RR_15!$B$240</f>
+        <v>153</v>
+      </c>
+      <c r="G18" s="1">
+        <f>Stride!$B$240</f>
+        <v>158.6</v>
+      </c>
+      <c r="J18">
+        <f>FIFO!$B$241</f>
+        <v>165.1</v>
+      </c>
+      <c r="K18">
+        <f>SJF!$B$241</f>
+        <v>109.2</v>
+      </c>
+      <c r="L18">
+        <f>PESJF!$B$241</f>
+        <v>101.3</v>
+      </c>
+      <c r="M18">
+        <f>RR_5!$B$241</f>
+        <v>208.3</v>
+      </c>
+      <c r="N18">
+        <f>RR_10!$B$241</f>
+        <v>190</v>
+      </c>
+      <c r="O18">
+        <f>RR_15!$B$241</f>
+        <v>183.8</v>
+      </c>
+      <c r="P18">
+        <f>Stride!$B$241</f>
+        <v>189.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>FIFO!B255</f>
         <v>141.30000000000001</v>
@@ -1036,28 +1511,56 @@
         <f>SJF!B255</f>
         <v>111.5</v>
       </c>
-      <c r="C19" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D19" s="1">
-        <f>FIFO!E255</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <f>FIFO!F255</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <f>FIFO!G255</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <f>FIFO!H255</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f>PESJF!$B$255</f>
+        <v>102.3</v>
+      </c>
+      <c r="D19">
+        <f>RR_5!$B$255</f>
+        <v>247.4</v>
+      </c>
+      <c r="E19">
+        <f>RR_10!$B$255</f>
+        <v>210.3</v>
+      </c>
+      <c r="F19">
+        <f>RR_15!$B$255</f>
+        <v>206.5</v>
+      </c>
+      <c r="G19">
+        <f>Stride!$B$255</f>
+        <v>237.6</v>
+      </c>
+      <c r="J19">
+        <f>FIFO!$B$256</f>
+        <v>177.4</v>
+      </c>
+      <c r="K19">
+        <f>SJF!$B$256</f>
+        <v>147.6</v>
+      </c>
+      <c r="L19">
+        <f>PESJF!$B$256</f>
+        <v>138.4</v>
+      </c>
+      <c r="M19">
+        <f>RR_5!$B$256</f>
+        <v>283.5</v>
+      </c>
+      <c r="N19">
+        <f>RR_10!$B$256</f>
+        <v>246.4</v>
+      </c>
+      <c r="O19">
+        <f>RR_15!$B$256</f>
+        <v>242.6</v>
+      </c>
+      <c r="P19">
+        <f>Stride!$B$256</f>
+        <v>273.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>FIFO!B270</f>
         <v>96.5</v>
@@ -1066,28 +1569,56 @@
         <f>SJF!B270</f>
         <v>71.3</v>
       </c>
-      <c r="C20">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
-      </c>
-      <c r="D20">
-        <f>FIFO!E270</f>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f>FIFO!F270</f>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f>FIFO!G270</f>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f>FIFO!H270</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <f>PESJF!$B$270</f>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="D20" s="1">
+        <f>RR_5!$B$270</f>
+        <v>156.19999999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <f>RR_10!$B$270</f>
+        <v>149.5</v>
+      </c>
+      <c r="F20" s="1">
+        <f>RR_15!$B$270</f>
+        <v>150.4</v>
+      </c>
+      <c r="G20" s="1">
+        <f>Stride!$B$270</f>
+        <v>172.8</v>
+      </c>
+      <c r="J20">
+        <f>FIFO!$B$271</f>
+        <v>125.2</v>
+      </c>
+      <c r="K20">
+        <f>SJF!$B$271</f>
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <f>PESJF!$B$271</f>
+        <v>97.1</v>
+      </c>
+      <c r="M20">
+        <f>RR_5!$B$271</f>
+        <v>184.9</v>
+      </c>
+      <c r="N20">
+        <f>RR_10!$B$271</f>
+        <v>178.2</v>
+      </c>
+      <c r="O20">
+        <f>RR_15!$B$271</f>
+        <v>179.1</v>
+      </c>
+      <c r="P20">
+        <f>Stride!$B$271</f>
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>FIFO!B285</f>
         <v>138.30000000000001</v>
@@ -1096,28 +1627,56 @@
         <f>SJF!B285</f>
         <v>62.5</v>
       </c>
-      <c r="C21" s="1">
-        <f>PESJF!$B$15</f>
-        <v>70.2</v>
-      </c>
-      <c r="D21" s="1">
-        <f>FIFO!E285</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <f>FIFO!F285</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <f>FIFO!G285</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <f>FIFO!H285</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f>PESJF!$B$285</f>
+        <v>62.2</v>
+      </c>
+      <c r="D21">
+        <f>RR_5!$B$285</f>
+        <v>139</v>
+      </c>
+      <c r="E21">
+        <f>RR_10!$B$285</f>
+        <v>162.1</v>
+      </c>
+      <c r="F21">
+        <f>RR_15!$B$285</f>
+        <v>152.6</v>
+      </c>
+      <c r="G21">
+        <f>Stride!$B$285</f>
+        <v>158.6</v>
+      </c>
+      <c r="J21">
+        <f>FIFO!$B$286</f>
+        <v>165.4</v>
+      </c>
+      <c r="K21">
+        <f>SJF!$B$286</f>
+        <v>89.6</v>
+      </c>
+      <c r="L21">
+        <f>PESJF!$B$286</f>
+        <v>89.3</v>
+      </c>
+      <c r="M21">
+        <f>RR_5!$B$286</f>
+        <v>166.1</v>
+      </c>
+      <c r="N21">
+        <f>RR_10!$B$286</f>
+        <v>189.2</v>
+      </c>
+      <c r="O21">
+        <f>RR_15!$B$286</f>
+        <v>179.7</v>
+      </c>
+      <c r="P21">
+        <f>Stride!$B$286</f>
+        <v>185.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>FIFO!B300</f>
         <v>156.6</v>
@@ -1127,24 +1686,52 @@
         <v>136</v>
       </c>
       <c r="C22">
-        <f>PESJF!$B$30</f>
-        <v>83.6</v>
+        <f>PESJF!$B$300</f>
+        <v>135.4</v>
       </c>
       <c r="D22">
-        <f>FIFO!E300</f>
-        <v>0</v>
+        <f>RR_5!$B$300</f>
+        <v>330.6</v>
       </c>
       <c r="E22">
-        <f>FIFO!F300</f>
-        <v>0</v>
+        <f>RR_10!$B$300</f>
+        <v>293.10000000000002</v>
       </c>
       <c r="F22">
-        <f>FIFO!G300</f>
-        <v>0</v>
+        <f>RR_15!$B$300</f>
+        <v>269.7</v>
       </c>
       <c r="G22">
-        <f>FIFO!H300</f>
-        <v>0</v>
+        <f>Stride!$B$300</f>
+        <v>308</v>
+      </c>
+      <c r="J22">
+        <f>FIFO!$B$301</f>
+        <v>198.7</v>
+      </c>
+      <c r="K22">
+        <f>SJF!$B$301</f>
+        <v>178.1</v>
+      </c>
+      <c r="L22">
+        <f>PESJF!$B$301</f>
+        <v>177.5</v>
+      </c>
+      <c r="M22">
+        <f>RR_5!$B$301</f>
+        <v>372.7</v>
+      </c>
+      <c r="N22">
+        <f>RR_10!$B$301</f>
+        <v>335.2</v>
+      </c>
+      <c r="O22">
+        <f>RR_15!$B$301</f>
+        <v>311.8</v>
+      </c>
+      <c r="P22">
+        <f>Stride!$B$301</f>
+        <v>350.1</v>
       </c>
     </row>
   </sheetData>
@@ -1157,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K301"/>
   <sheetViews>
-    <sheetView topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
this should be the updated graph file
</commit_message>
<xml_diff>
--- a/Graph_FIle.xlsx
+++ b/Graph_FIle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="50">
   <si>
     <t>FIFO Test Results</t>
   </si>
@@ -169,6 +169,9 @@
   <si>
     <t>Turn Around Times</t>
   </si>
+  <si>
+    <t>JOB</t>
+  </si>
 </sst>
 </file>
 
@@ -225,6 +228,1551 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Wait Times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>114.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>122.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>177.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>179.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>136.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>143.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>146.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>134.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>141.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>138.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>156.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SJF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>70.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>105.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>78.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>111.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PESJF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>70.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>73.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>102.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>68.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>135.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>163.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>217.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>136.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>265.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>164.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>175.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>221.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>185.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>213.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>177.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>247.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>156.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>330.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>152.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>189.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>123.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>232.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>145.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>201.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>210.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>162.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>293.10000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>146.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>139.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>291.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>291.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>212.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>149.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>148.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>158.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>194.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>206.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>150.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>152.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>269.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stride</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>162.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>216.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>154.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>343.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>225.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>178.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>201.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>158.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>237.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>158.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="9351552"/>
+        <c:axId val="9353088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="9351552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="9353088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9353088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Clock Ticks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="9351552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Turnaround Times </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>145.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>222.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>169.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>144.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>145.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>174.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>139.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>165.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>177.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>125.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>165.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>198.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SJF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>188.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>188.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>122.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>109.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>147.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>178.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PESJF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>101.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>222.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>104.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>115.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>128.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>101.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>138.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>177.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>194.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>248.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>204.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>355.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>298.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>206.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>248.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>283.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>184.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>166.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>372.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$3:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>183.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>162.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>363.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>358.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>265.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>183.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>170.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>232.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>190.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>244.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>246.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>178.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>189.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>335.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RR_15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>177.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>148.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>167.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>335.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>334.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>245.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>178.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>173.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>189.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>209.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>189.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>229.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>183.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>242.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>179.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>179.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>311.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stride</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$Q$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>193.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>224.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>183.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>387.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>258.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>194.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>209.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>218.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>218.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>236.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>189.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>273.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>201.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>185.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>350.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="155358720"/>
+        <c:axId val="155360256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="155358720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Test Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="155360256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="155360256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Clock Ticks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="155358720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,1222 +2062,1348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
       <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>45</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>47</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <f>FIFO!B15</f>
         <v>114.2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <f>SJF!B15</f>
         <v>70.099999999999994</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <f>PESJF!$B$15</f>
         <v>70.2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <f>RR_5!$B$15</f>
         <v>163.30000000000001</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <f>RR_10!$B$15</f>
         <v>152.69999999999999</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <f>RR_15!$B$15</f>
         <v>146.6</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <f>Stride!$B$15</f>
         <v>162.30000000000001</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <f>FIFO!$B$16</f>
         <v>145.1</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>SJF!$B$16</f>
         <v>101</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>PESJF!$B$16</f>
         <v>101.1</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f>RR_5!$B$16</f>
         <v>194.2</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <f>RR_10!$B$16</f>
         <v>183.6</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <f>RR_15!$B$16</f>
         <v>177.5</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <f>Stride!$B$16</f>
         <v>193.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <f>FIFO!B30</f>
         <v>134.6</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <f>SJF!B30</f>
         <v>90.8</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f>PESJF!$B$30</f>
         <v>83.6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>RR_5!$B$30</f>
         <v>217.7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f>RR_10!$B$30</f>
         <v>189.5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f>RR_15!$B$30</f>
         <v>184</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f>Stride!$B$30</f>
         <v>184.3</v>
       </c>
       <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
         <f>FIFO!$B$31</f>
         <v>165.3</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>SJF!$B$31</f>
         <v>121.5</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>PESJF!$B$31</f>
         <v>114.3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f>RR_5!$B$31</f>
         <v>248.4</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <f>RR_10!$B$31</f>
         <v>220.2</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f>RR_15!$B$31</f>
         <v>214.7</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f>Stride!$B$31</f>
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <f>FIFO!B45</f>
         <v>110.6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <f>SJF!B45</f>
         <v>76.5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <f>PESJF!$B$45</f>
         <v>74.400000000000006</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <f>RR_5!$B$45</f>
         <v>174.2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <f>RR_10!$B$45</f>
         <v>164.1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <f>RR_15!$B$45</f>
         <v>153.4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f>Stride!$B$45</f>
         <v>216.8</v>
       </c>
       <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
         <f>FIFO!$B$46</f>
         <v>140.80000000000001</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f>SJF!$B$46</f>
         <v>106.7</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>PESJF!$B$46</f>
         <v>104.6</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f>RR_5!$B$46</f>
         <v>204.4</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f>RR_10!$B$46</f>
         <v>194.3</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f>RR_15!$B$46</f>
         <v>183.6</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f>Stride!$B$46</f>
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <f>FIFO!B60</f>
         <v>72.7</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <f>SJF!B60</f>
         <v>64.7</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <f>PESJF!$B$60</f>
         <v>63.8</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>RR_5!$B$60</f>
         <v>147</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f>RR_10!$B$60</f>
         <v>133.6</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f>RR_15!$B$60</f>
         <v>119.8</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f>Stride!$B$60</f>
         <v>195.4</v>
       </c>
       <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
         <f>FIFO!$B$61</f>
         <v>101.8</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>SJF!$B$61</f>
         <v>93.8</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>PESJF!$B$61</f>
         <v>92.9</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f>RR_5!$B$61</f>
         <v>176.1</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f>RR_10!$B$61</f>
         <v>162.69999999999999</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f>RR_15!$B$61</f>
         <v>148.9</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f>Stride!$B$61</f>
         <v>224.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <f>FIFO!B75</f>
         <v>122.4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <f>SJF!B75</f>
         <v>76.8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <f>PESJF!$B$75</f>
         <v>64.900000000000006</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <f>RR_5!$B$75</f>
         <v>148.5</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <f>RR_10!$B$75</f>
         <v>146.9</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <f>RR_15!$B$75</f>
         <v>139.6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <f>Stride!$B$75</f>
         <v>154.9</v>
       </c>
       <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
         <f>FIFO!$B$76</f>
         <v>150.6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>SJF!$B$76</f>
         <v>105</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>PESJF!$B$76</f>
         <v>93.1</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f>RR_5!$B$76</f>
         <v>176.7</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f>RR_10!$B$76</f>
         <v>175.1</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f>RR_15!$B$76</f>
         <v>167.8</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f>Stride!$B$76</f>
         <v>183.1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <f>FIFO!B90</f>
         <v>177.9</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <f>SJF!B90</f>
         <v>145.19999999999999</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <f>PESJF!$B$90</f>
         <v>140.9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <f>RR_5!$B$90</f>
         <v>318.39999999999998</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <f>RR_10!$B$90</f>
         <v>320.10000000000002</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <f>RR_15!$B$90</f>
         <v>291.60000000000002</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <f>Stride!$B$90</f>
         <v>343.8</v>
       </c>
       <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
         <f>FIFO!$B$91</f>
         <v>221.5</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f>SJF!$B$91</f>
         <v>188.8</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>PESJF!$B$91</f>
         <v>184.5</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f>RR_5!$B$91</f>
         <v>362</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f>RR_10!$B$91</f>
         <v>363.7</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f>RR_15!$B$91</f>
         <v>335.2</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f>Stride!$B$91</f>
         <v>387.4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
         <f>FIFO!B105</f>
         <v>179.6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <f>SJF!B105</f>
         <v>145</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <f>PESJF!$B$105</f>
         <v>143</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>RR_5!$B$105</f>
         <v>312.3</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f>RR_10!$B$105</f>
         <v>315</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f>RR_15!$B$105</f>
         <v>291.7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f>Stride!$B$105</f>
         <v>331.9</v>
       </c>
       <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
         <f>FIFO!$B$106</f>
         <v>222.8</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f>SJF!$B$106</f>
         <v>188.2</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>FIFO!$B$106</f>
         <v>222.8</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f>RR_5!$B$106</f>
         <v>355.5</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f>RR_10!$B$106</f>
         <v>358.2</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f>RR_15!$B$106</f>
         <v>334.9</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f>Stride!$B$106</f>
         <v>375.1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <f>FIFO!B120</f>
         <v>90.9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <f>SJF!B120</f>
         <v>55.3</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <f>PESJF!$B$120</f>
         <v>54.5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <f>RR_5!$B$120</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <f>RR_10!$B$120</f>
         <v>123.8</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <f>RR_15!$B$120</f>
         <v>110.4</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <f>Stride!$B$120</f>
         <v>148.9</v>
       </c>
       <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
         <f>FIFO!$B$121</f>
         <v>117.9</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f>SJF!$B$121</f>
         <v>82.3</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f>PESJF!$B$121</f>
         <v>81.5</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f>RR_5!$B$121</f>
         <v>163.80000000000001</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <f>RR_10!$B$121</f>
         <v>150.80000000000001</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <f>RR_15!$B$121</f>
         <v>137.4</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f>Stride!$B$121</f>
         <v>175.9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
         <f>FIFO!B135</f>
         <v>136.4</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <f>SJF!B135</f>
         <v>104.2</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f>PESJF!$B$135</f>
         <v>104.3</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f>RR_5!$B$135</f>
         <v>265.3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f>RR_10!$B$135</f>
         <v>232.3</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f>RR_15!$B$135</f>
         <v>212.8</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f>Stride!$B$135</f>
         <v>225.3</v>
       </c>
       <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
         <f>FIFO!$B$136</f>
         <v>169.3</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f>SJF!$B$136</f>
         <v>137.1</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f>PESJF!$B$136</f>
         <v>137.19999999999999</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f>RR_5!$B$136</f>
         <v>298.2</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f>RR_10!$B$136</f>
         <v>265.2</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <f>RR_15!$B$136</f>
         <v>245.7</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f>Stride!$B$136</f>
         <v>258.2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <f>FIFO!B150</f>
         <v>101.1</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <f>SJF!B150</f>
         <v>72</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <f>PESJF!$B$150</f>
         <v>74</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <f>RR_5!$B$150</f>
         <v>164.1</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <f>RR_10!$B$150</f>
         <v>154.9</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <f>RR_15!$B$150</f>
         <v>149.4</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <f>Stride!$B$150</f>
         <v>165.2</v>
       </c>
       <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
         <f>FIFO!$B$151</f>
         <v>130</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f>SJF!$B$151</f>
         <v>100.9</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>PESJF!$B$151</f>
         <v>102.9</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>RR_5!$B$151</f>
         <v>193</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <f>RR_10!$B$151</f>
         <v>183.8</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <f>RR_15!$B$151</f>
         <v>178.3</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <f>Stride!$B$151</f>
         <v>194.1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
         <f>FIFO!B165</f>
         <v>119.5</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <f>SJF!B165</f>
         <v>62.7</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <f>PESJF!$B$165</f>
         <v>62</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f>RR_5!$B$165</f>
         <v>128.30000000000001</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f>RR_10!$B$165</f>
         <v>145.69999999999999</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f>RR_15!$B$165</f>
         <v>148.69999999999999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f>Stride!$B$165</f>
         <v>133.1</v>
       </c>
       <c r="J13">
+        <v>11</v>
+      </c>
+      <c r="K13">
         <f>FIFO!$B$166</f>
         <v>144.6</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f>SJF!$B$166</f>
         <v>87.8</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f>PESJF!$B$166</f>
         <v>87.1</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f>RR_5!$B$166</f>
         <v>153.4</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <f>RR_10!$B$166</f>
         <v>170.8</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <f>RR_15!$B$166</f>
         <v>173.8</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <f>Stride!$B$166</f>
         <v>158.19999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <f>FIFO!B180</f>
         <v>114.9</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <f>SJF!B180</f>
         <v>85.2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <f>PESJF!$B$180</f>
         <v>73.900000000000006</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <f>RR_5!$B$180</f>
         <v>175.2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <f>RR_10!$B$180</f>
         <v>176</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <f>RR_15!$B$180</f>
         <v>158.80000000000001</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <f>Stride!$B$180</f>
         <v>178.8</v>
       </c>
       <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
         <f>FIFO!$B$181</f>
         <v>145.9</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f>SJF!$B$181</f>
         <v>116.2</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f>PESJF!$B$181</f>
         <v>104.9</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f>RR_5!$B$181</f>
         <v>206.2</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <f>RR_10!$B$181</f>
         <v>207</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <f>RR_15!$B$181</f>
         <v>189.8</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <f>Stride!$B$181</f>
         <v>209.8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
         <f>FIFO!B195</f>
         <v>143.69999999999999</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <f>SJF!B195</f>
         <v>91.6</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <f>PESJF!$B$195</f>
         <v>84.4</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f>RR_5!$B$195</f>
         <v>221.1</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f>RR_10!$B$195</f>
         <v>201.5</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <f>RR_15!$B$195</f>
         <v>178.2</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f>Stride!$B$195</f>
         <v>188</v>
       </c>
       <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15">
         <f>FIFO!$B$196</f>
         <v>174.6</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f>SJF!$B$196</f>
         <v>122.5</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f>PESJF!$B$196</f>
         <v>115.3</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <f>RR_5!$B$196</f>
         <v>252</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <f>RR_10!$B$196</f>
         <v>232.4</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <f>RR_15!$B$196</f>
         <v>209.1</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <f>Stride!$B$196</f>
         <v>218.9</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <f>FIFO!B210</f>
         <v>111</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <f>SJF!B210</f>
         <v>85.6</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <f>PESJF!$B$210</f>
         <v>71.900000000000006</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <f>RR_5!$B$210</f>
         <v>185.4</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f>RR_10!$B$210</f>
         <v>161.80000000000001</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <f>RR_15!$B$210</f>
         <v>161.1</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <f>Stride!$B$210</f>
         <v>190</v>
       </c>
       <c r="J16">
+        <v>14</v>
+      </c>
+      <c r="K16">
         <f>FIFO!$B$211</f>
         <v>139.6</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <f>SJF!$B$211</f>
         <v>114.2</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f>PESJF!$B$211</f>
         <v>100.5</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <f>RR_5!$B$211</f>
         <v>214</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <f>RR_10!$B$211</f>
         <v>190.4</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <f>RR_15!$B$211</f>
         <v>189.7</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <f>Stride!$B$211</f>
         <v>218.6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
         <f>FIFO!B225</f>
         <v>146.69999999999999</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <f>SJF!B225</f>
         <v>105.7</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <f>PESJF!$B$225</f>
         <v>93.4</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f>RR_5!$B$225</f>
         <v>213.7</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f>RR_10!$B$225</f>
         <v>209</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f>RR_15!$B$225</f>
         <v>194.3</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f>Stride!$B$225</f>
         <v>201.4</v>
       </c>
       <c r="J17">
+        <v>15</v>
+      </c>
+      <c r="K17">
         <f>FIFO!$B$226</f>
         <v>181.9</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <f>SJF!$B$226</f>
         <v>140.9</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f>PESJF!$B$226</f>
         <v>128.6</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <f>RR_5!$B$226</f>
         <v>248.9</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <f>RR_10!$B$226</f>
         <v>244.2</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <f>RR_15!$B$226</f>
         <v>229.5</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <f>Stride!$B$226</f>
         <v>236.6</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
         <f>FIFO!B240</f>
         <v>134.30000000000001</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <f>SJF!B240</f>
         <v>78.400000000000006</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <f>PESJF!$B$240</f>
         <v>70.5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <f>RR_5!$B$240</f>
         <v>177.5</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f>RR_10!$B$240</f>
         <v>159.19999999999999</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <f>RR_15!$B$240</f>
         <v>153</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f>Stride!$B$240</f>
         <v>158.6</v>
       </c>
       <c r="J18">
+        <v>16</v>
+      </c>
+      <c r="K18">
         <f>FIFO!$B$241</f>
         <v>165.1</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <f>SJF!$B$241</f>
         <v>109.2</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f>PESJF!$B$241</f>
         <v>101.3</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <f>RR_5!$B$241</f>
         <v>208.3</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <f>RR_10!$B$241</f>
         <v>190</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <f>RR_15!$B$241</f>
         <v>183.8</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <f>Stride!$B$241</f>
         <v>189.4</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
         <f>FIFO!B255</f>
         <v>141.30000000000001</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <f>SJF!B255</f>
         <v>111.5</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <f>PESJF!$B$255</f>
         <v>102.3</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f>RR_5!$B$255</f>
         <v>247.4</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f>RR_10!$B$255</f>
         <v>210.3</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <f>RR_15!$B$255</f>
         <v>206.5</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f>Stride!$B$255</f>
         <v>237.6</v>
       </c>
       <c r="J19">
+        <v>17</v>
+      </c>
+      <c r="K19">
         <f>FIFO!$B$256</f>
         <v>177.4</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <f>SJF!$B$256</f>
         <v>147.6</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f>PESJF!$B$256</f>
         <v>138.4</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f>RR_5!$B$256</f>
         <v>283.5</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <f>RR_10!$B$256</f>
         <v>246.4</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f>RR_15!$B$256</f>
         <v>242.6</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <f>Stride!$B$256</f>
         <v>273.7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
         <f>FIFO!B270</f>
         <v>96.5</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <f>SJF!B270</f>
         <v>71.3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <f>PESJF!$B$270</f>
         <v>68.400000000000006</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <f>RR_5!$B$270</f>
         <v>156.19999999999999</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <f>RR_10!$B$270</f>
         <v>149.5</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <f>RR_15!$B$270</f>
         <v>150.4</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <f>Stride!$B$270</f>
         <v>172.8</v>
       </c>
       <c r="J20">
+        <v>18</v>
+      </c>
+      <c r="K20">
         <f>FIFO!$B$271</f>
         <v>125.2</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <f>SJF!$B$271</f>
         <v>100</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f>PESJF!$B$271</f>
         <v>97.1</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <f>RR_5!$B$271</f>
         <v>184.9</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <f>RR_10!$B$271</f>
         <v>178.2</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <f>RR_15!$B$271</f>
         <v>179.1</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <f>Stride!$B$271</f>
         <v>201.5</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
         <f>FIFO!B285</f>
         <v>138.30000000000001</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <f>SJF!B285</f>
         <v>62.5</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <f>PESJF!$B$285</f>
         <v>62.2</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <f>RR_5!$B$285</f>
         <v>139</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f>RR_10!$B$285</f>
         <v>162.1</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <f>RR_15!$B$285</f>
         <v>152.6</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f>Stride!$B$285</f>
         <v>158.6</v>
       </c>
       <c r="J21">
+        <v>19</v>
+      </c>
+      <c r="K21">
         <f>FIFO!$B$286</f>
         <v>165.4</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <f>SJF!$B$286</f>
         <v>89.6</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f>PESJF!$B$286</f>
         <v>89.3</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <f>RR_5!$B$286</f>
         <v>166.1</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <f>RR_10!$B$286</f>
         <v>189.2</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <f>RR_15!$B$286</f>
         <v>179.7</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <f>Stride!$B$286</f>
         <v>185.7</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
         <f>FIFO!B300</f>
         <v>156.6</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <f>SJF!B300</f>
         <v>136</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <f>PESJF!$B$300</f>
         <v>135.4</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <f>RR_5!$B$300</f>
         <v>330.6</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <f>RR_10!$B$300</f>
         <v>293.10000000000002</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <f>RR_15!$B$300</f>
         <v>269.7</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f>Stride!$B$300</f>
         <v>308</v>
       </c>
       <c r="J22">
+        <v>20</v>
+      </c>
+      <c r="K22">
         <f>FIFO!$B$301</f>
         <v>198.7</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <f>SJF!$B$301</f>
         <v>178.1</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f>PESJF!$B$301</f>
         <v>177.5</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <f>RR_5!$B$301</f>
         <v>372.7</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <f>RR_10!$B$301</f>
         <v>335.2</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <f>RR_15!$B$301</f>
         <v>311.8</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <f>Stride!$B$301</f>
         <v>350.1</v>
       </c>
@@ -1737,6 +3411,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>